<commit_message>
Updates/bugfixes while running pilot-04.
</commit_message>
<xml_diff>
--- a/Muscle_Response_Times.xlsx
+++ b/Muscle_Response_Times.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyRepos\NML-NHP\Mouse_SCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyRepos\NML\Mouse_SCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB5484B-D50F-4494-8BCE-3D38702EF18B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F2E18C-DE2B-4BA5-9CA3-798BB63AECD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11328" yWindow="2400" windowWidth="14280" windowHeight="9636" xr2:uid="{21034878-75EC-4AEB-A868-4199A65C7D41}"/>
+    <workbookView xWindow="31035" yWindow="2430" windowWidth="21600" windowHeight="11385" xr2:uid="{21034878-75EC-4AEB-A868-4199A65C7D41}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -481,16 +481,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816DACA5-D80E-497E-9F77-77E41F063443}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -512,139 +512,139 @@
         <v>3.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>8.4999999999999995E-4</v>
+        <v>2E-3</v>
       </c>
       <c r="C3">
-        <v>2.7499999999999998E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>3.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>8.4999999999999995E-4</v>
+        <v>2E-3</v>
       </c>
       <c r="C4">
-        <v>2.7499999999999998E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>3.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5">
-        <v>8.4999999999999995E-4</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="C5">
-        <v>2.7499999999999998E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>3.2000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6">
-        <v>8.4999999999999995E-4</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="C6">
-        <v>2.7499999999999998E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>3.2000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1.15E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="C7">
-        <v>3.2000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1.15E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="C8">
-        <v>3.2000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1.6000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="C9">
-        <v>3.3E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>1.6000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="C10">
-        <v>3.3E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>2.3500000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C11">
-        <v>4.4000000000000003E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>2.3500000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C12">
-        <v>4.4000000000000003E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>2.3500000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C13">
-        <v>4.4000000000000003E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>2.3500000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C14">
-        <v>4.4000000000000003E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -652,10 +652,10 @@
         <v>8.4999999999999995E-4</v>
       </c>
       <c r="C15">
-        <v>3.5000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -663,7 +663,7 @@
         <v>8.4999999999999995E-4</v>
       </c>
       <c r="C16">
-        <v>3.5000000000000001E-3</v>
+        <v>4.4999999999999997E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes from after the 2024-07-02 procedure.
</commit_message>
<xml_diff>
--- a/Muscle_Response_Times.xlsx
+++ b/Muscle_Response_Times.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyRepos\NML\Mouse_SCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F2E18C-DE2B-4BA5-9CA3-798BB63AECD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0F9EC8-5C3A-45D6-BE55-5D8217ACB3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31035" yWindow="2430" windowWidth="21600" windowHeight="11385" xr2:uid="{21034878-75EC-4AEB-A868-4199A65C7D41}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{21034878-75EC-4AEB-A868-4199A65C7D41}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -482,7 +482,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +506,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>8.4999999999999995E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="C2">
         <v>3.5000000000000001E-3</v>
@@ -517,7 +517,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C3">
         <v>3.5000000000000001E-3</v>
@@ -528,7 +528,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C4">
         <v>3.5000000000000001E-3</v>
@@ -539,10 +539,10 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>2.2000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C5">
-        <v>3.2000000000000002E-3</v>
+        <v>3.5000000000000001E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -550,10 +550,10 @@
         <v>17</v>
       </c>
       <c r="B6">
-        <v>2.2000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C6">
-        <v>3.2000000000000002E-3</v>
+        <v>3.5000000000000001E-3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -561,10 +561,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C7">
-        <v>4.4999999999999997E-3</v>
+        <v>2.2000000000000001E-3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -572,10 +572,10 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C8">
-        <v>4.4999999999999997E-3</v>
+        <v>2.2000000000000001E-3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -583,10 +583,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C9">
-        <v>4.4999999999999997E-3</v>
+        <v>2.2000000000000001E-3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -594,10 +594,10 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C10">
-        <v>4.4999999999999997E-3</v>
+        <v>2.2000000000000001E-3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -605,10 +605,10 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>3.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C11">
-        <v>6.0000000000000001E-3</v>
+        <v>3.5000000000000001E-3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -616,10 +616,10 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>3.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C12">
-        <v>6.0000000000000001E-3</v>
+        <v>3.5000000000000001E-3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -627,10 +627,10 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>3.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C13">
-        <v>6.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -638,10 +638,10 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>3.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C14">
-        <v>6.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -649,10 +649,10 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>8.4999999999999995E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="C15">
-        <v>4.4999999999999997E-3</v>
+        <v>3.5000000000000001E-3</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -660,10 +660,10 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>8.4999999999999995E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="C16">
-        <v>4.4999999999999997E-3</v>
+        <v>3.5000000000000001E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates after post-processing from 2024-07-02 procedure.
</commit_message>
<xml_diff>
--- a/Muscle_Response_Times.xlsx
+++ b/Muscle_Response_Times.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyRepos\NML\Mouse_SCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0F9EC8-5C3A-45D6-BE55-5D8217ACB3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890B672B-9712-4F49-8BC6-60FE9D98E026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{21034878-75EC-4AEB-A868-4199A65C7D41}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{21034878-75EC-4AEB-A868-4199A65C7D41}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Muscle</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>L-P-DELTOID</t>
+  </si>
+  <si>
+    <t>PolynomialOrder</t>
   </si>
 </sst>
 </file>
@@ -142,9 +145,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,18 +488,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816DACA5-D80E-497E-9F77-77E41F063443}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,8 +510,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -511,8 +524,11 @@
       <c r="C2">
         <v>3.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -520,10 +536,13 @@
         <v>1E-3</v>
       </c>
       <c r="C3">
-        <v>3.5000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -531,10 +550,13 @@
         <v>1E-3</v>
       </c>
       <c r="C4">
-        <v>3.5000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -542,10 +564,13 @@
         <v>1E-3</v>
       </c>
       <c r="C5">
-        <v>3.5000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -553,32 +578,41 @@
         <v>1E-3</v>
       </c>
       <c r="C6">
-        <v>3.5000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1E-3</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="C7">
-        <v>2.2000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2E-3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1E-3</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="C8">
-        <v>2.2000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2E-3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -586,10 +620,13 @@
         <v>1E-3</v>
       </c>
       <c r="C9">
-        <v>2.2000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2E-3</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -597,54 +634,69 @@
         <v>1E-3</v>
       </c>
       <c r="C10">
-        <v>2.2000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2E-3</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1E-3</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="C11">
-        <v>3.5000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2E-3</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1E-3</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="C12">
-        <v>3.5000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2E-3</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>1E-3</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="C13">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>1E-3</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="C14">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -654,8 +706,11 @@
       <c r="C15">
         <v>3.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -664,6 +719,9 @@
       </c>
       <c r="C16">
         <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="D16" s="3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>